<commit_message>
Task [15] Separate counts for all and specific emotions.
	- Improve regex in reaction words.
	- Overall counts. Update boxes for overall. Separate counts.
	- Specific counts. Update boxes for specific emotions. Separate counts.
</commit_message>
<xml_diff>
--- a/R/final-list-of-emoticons.xlsx
+++ b/R/final-list-of-emoticons.xlsx
@@ -111,66 +111,15 @@
     <t>&lt;U+00B8&gt;&lt;U+0098&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0097&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0099&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+009A&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+008B&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+009C&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+009D&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+009B&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B4&gt;&lt;U+0091&gt; </t>
-  </si>
-  <si>
     <t>&lt;U+00B4&gt;&lt;U+0097&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;U+00B4&gt;&lt;U+0093&gt; </t>
-  </si>
-  <si>
     <t>&lt;U+00B8&gt;&lt;U+008E&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0082&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B1&gt;&lt;U+008C&gt; </t>
-  </si>
-  <si>
     <t>&lt;U+00B1&gt;&lt;U+008D&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00AC&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00B8&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00B9&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00BA&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00BC&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00BD&gt; </t>
-  </si>
-  <si>
     <t>:/</t>
   </si>
   <si>
@@ -180,60 +129,12 @@
     <t>:poop:</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;U+00B2&gt;&lt;U+00A9&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B4&gt;&lt;U+00A2&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+008F&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0091&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0092&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0095&gt; </t>
-  </si>
-  <si>
-    <t>&lt;U+00B1&gt;&lt;U+008E&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0090&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00A6&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00B7&gt; </t>
-  </si>
-  <si>
     <t>&gt;:(</t>
   </si>
   <si>
     <t>3:)</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00A4&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0088&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B1&gt;&lt;U+00BF&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00A0&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00A1&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00BE&gt; </t>
-  </si>
-  <si>
     <t>:P</t>
   </si>
   <si>
@@ -249,70 +150,169 @@
     <t>&lt;U+00B8&gt;&lt;U+00AD&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0093&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0094&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+0096&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+009E&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+009F&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00A2&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00A3&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00A5&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00A9&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00AA&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00AB&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00BF&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B9&gt;&lt;U+0080&gt; </t>
-  </si>
-  <si>
     <t>o.O</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00A7&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00A8&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00B0&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00B1&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00AE&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00AF&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00B2&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;U+00B8&gt;&lt;U+00B3&gt; </t>
+    <t>&lt;U+00B2&gt;&lt;U+00A9&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B4&gt;&lt;U+00A2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+008F&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0091&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0092&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0095&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B1&gt;&lt;U+008E&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0090&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00A6&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00B7&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00A7&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00A8&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00B0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00B1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00AE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00AF&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00B2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00B3&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00A4&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0088&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B1&gt;&lt;U+00BF&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00A0&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00A1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00BE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0093&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0094&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0096&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+009E&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+009F&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00A2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00A3&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00A5&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00A9&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00AA&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00AB&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00BF&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B9&gt;&lt;U+0080&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+009A&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0097&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0099&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+008B&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+009C&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+009D&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+009B&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B4&gt;&lt;U+0091&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B4&gt;&lt;U+0093&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+0082&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B1&gt;&lt;U+008C&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00AC&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00B8&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00B9&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00BA&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00BC&gt;</t>
+  </si>
+  <si>
+    <t>&lt;U+00B8&gt;&lt;U+00BD&gt;</t>
   </si>
 </sst>
 </file>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,16 +699,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -716,16 +716,16 @@
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -733,16 +733,16 @@
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -750,16 +750,16 @@
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -767,16 +767,16 @@
         <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -784,16 +784,16 @@
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -801,16 +801,16 @@
         <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -818,16 +818,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -835,16 +835,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -852,10 +852,10 @@
         <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -863,10 +863,10 @@
         <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -874,10 +874,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,10 +885,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -896,10 +896,10 @@
         <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -907,7 +907,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -915,110 +915,110 @@
         <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Improvements] Add more words
</commit_message>
<xml_diff>
--- a/R/final-list-of-emoticons.xlsx
+++ b/R/final-list-of-emoticons.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="emoticons" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
   <si>
     <t>HAPPY</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>&lt;U+00B8&gt;&lt;U+00BD&gt;</t>
+  </si>
+  <si>
+    <t>=P</t>
   </si>
 </sst>
 </file>
@@ -368,12 +371,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,6 +1075,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>